<commit_message>
30 Jan 25 Updates Completed pad view
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wscsurtech\OneDrive - ConocoPhillips\Surveillance Technician\Tech Folders\Nick\DT\DT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{57FE8D54-CDDC-4370-80E3-F44FF3F6CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{003793E1-F831-4207-B905-B08291F6BA5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="2835" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>Formation enter</t>
   </si>
@@ -912,7 +912,7 @@
   <dimension ref="A2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,6 +963,9 @@
       <c r="D5" t="s">
         <v>53</v>
       </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
       <c r="M5" t="s">
         <v>48</v>
       </c>
@@ -1024,6 +1027,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
       <c r="B10">
         <v>3.6</v>
       </c>
@@ -1138,6 +1144,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
       <c r="B19">
         <v>3.15</v>
       </c>
@@ -1157,6 +1166,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
       <c r="B21">
         <v>3.17</v>
       </c>
@@ -1466,15 +1478,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
@@ -1482,6 +1485,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1504,14 +1516,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1519,4 +1523,12 @@
     <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
31 Jan 25 Updates
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wscsurtech\OneDrive - ConocoPhillips\Surveillance Technician\Tech Folders\Nick\DT\DT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8634654B-AAC3-4F77-85AB-5179FD51DE53}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="2835" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="2130" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -274,8 +274,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -303,9 +311,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,7 +921,7 @@
   <dimension ref="A2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,9 +1093,10 @@
       <c r="L13" t="s">
         <v>30</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1098,7 +1108,7 @@
       <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1478,6 +1488,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
@@ -1485,15 +1504,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1516,6 +1526,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1523,12 +1541,4 @@
     <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
2 Feb 25 Updates
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8634654B-AAC3-4F77-85AB-5179FD51DE53}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0BD3E0C-764A-401A-8BF4-A35D699EBEB4}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2130" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11235" yWindow="2385" windowWidth="23130" windowHeight="16920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
   <si>
     <t>Formation enter</t>
   </si>
@@ -268,6 +268,30 @@
   </si>
   <si>
     <t>Add offset well button</t>
+  </si>
+  <si>
+    <t>Plan vs Actual window</t>
+  </si>
+  <si>
+    <t>Update actual window</t>
+  </si>
+  <si>
+    <t>Update plan window</t>
+  </si>
+  <si>
+    <t>Modify importCsv.py to set as plan in databse</t>
+  </si>
+  <si>
+    <t>Update database to have planned vs actual column</t>
+  </si>
+  <si>
+    <t>Multilateral wells</t>
+  </si>
+  <si>
+    <t>3.23.1</t>
+  </si>
+  <si>
+    <t>Under update directional have a add lateral button</t>
   </si>
 </sst>
 </file>
@@ -918,10 +942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058DFC1C-49F3-4496-A186-6E8CEF18F5C9}">
-  <dimension ref="A2:N21"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1155,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1142,7 +1166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1153,7 +1177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1164,7 +1188,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -1175,7 +1199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1184,6 +1208,62 @@
       </c>
       <c r="C21" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>3.18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>3.19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3.21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>3.22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3.23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1488,15 +1568,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
@@ -1504,6 +1575,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1526,14 +1606,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1541,4 +1613,12 @@
     <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
9 Feb 25 Updates
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0BD3E0C-764A-401A-8BF4-A35D699EBEB4}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78EE511-BB3C-454E-97DE-D5BD4D6EF60E}"/>
   <bookViews>
-    <workbookView xWindow="11235" yWindow="2385" windowWidth="23130" windowHeight="16920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="3630" windowWidth="29880" windowHeight="14295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>Formation enter</t>
   </si>
@@ -291,7 +291,10 @@
     <t>3.23.1</t>
   </si>
   <si>
-    <t>Under update directional have a add lateral button</t>
+    <t>TVD vs MD plot</t>
+  </si>
+  <si>
+    <t>Under update directional have an add lateral button</t>
   </si>
 </sst>
 </file>
@@ -942,10 +945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058DFC1C-49F3-4496-A186-6E8CEF18F5C9}">
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,6 +1266,17 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>3.24</v>
+      </c>
+      <c r="C29" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
9 Feb 2025 Update
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78EE511-BB3C-454E-97DE-D5BD4D6EF60E}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5AFF306-D9B4-41BB-996F-F9B64FE9B157}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3630" windowWidth="29880" windowHeight="14295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="1260" windowWidth="19035" windowHeight="19230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>Formation enter</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Verify north south east and west are labled correctly on 3d plot</t>
   </si>
   <si>
-    <t>Tree Widget?</t>
-  </si>
-  <si>
     <t>Size of chart needs to be bigger 3S-714 example plan view</t>
   </si>
   <si>
@@ -295,6 +292,45 @@
   </si>
   <si>
     <t>Under update directional have an add lateral button</t>
+  </si>
+  <si>
+    <t>3.23.2</t>
+  </si>
+  <si>
+    <t>Add planed or actual radio putton to latter name window</t>
+  </si>
+  <si>
+    <t>3.23.3</t>
+  </si>
+  <si>
+    <t>Change names in annotations to inclue lateral if not Null</t>
+  </si>
+  <si>
+    <t>Build main GUI window with buttons to add different types of casing</t>
+  </si>
+  <si>
+    <t>Build matplotlib window to show well diagram</t>
+  </si>
+  <si>
+    <t>Build database to hold casing sizes for each well</t>
+  </si>
+  <si>
+    <t>Build window that shows casing information for each section</t>
+  </si>
+  <si>
+    <t>Surface casing</t>
+  </si>
+  <si>
+    <t>Intermediate Casing</t>
+  </si>
+  <si>
+    <t>Liners</t>
+  </si>
+  <si>
+    <t>Production casing</t>
+  </si>
+  <si>
+    <t>Upper completions</t>
   </si>
 </sst>
 </file>
@@ -879,7 +915,7 @@
         <v>1.5</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,7 +926,7 @@
         <v>1.6</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +971,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -945,10 +981,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058DFC1C-49F3-4496-A186-6E8CEF18F5C9}">
-  <dimension ref="A2:N29"/>
+  <dimension ref="A2:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1100,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>3.6</v>
@@ -1081,7 +1117,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B11">
         <v>3.7</v>
@@ -1095,7 +1131,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>3.8</v>
@@ -1115,7 +1151,7 @@
         <v>3.9</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
         <v>30</v>
@@ -1133,18 +1169,18 @@
         <v>3.1</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="2">
         <v>3.11</v>
       </c>
-      <c r="C15" t="s">
-        <v>67</v>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1155,7 +1191,7 @@
         <v>3.12</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1166,7 +1202,7 @@
         <v>3.13</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,18 +1213,18 @@
         <v>3.14</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>3.15</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,58 +1235,73 @@
         <v>3.16</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <v>3.17</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
       <c r="B22">
         <v>3.18</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
       <c r="B23">
         <v>3.19</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
       <c r="B24" s="1">
         <v>3.2</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
       <c r="B25">
         <v>3.21</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
       <c r="B26">
         <v>3.22</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,26 +1309,45 @@
         <v>3.23</v>
       </c>
       <c r="C27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31">
+        <v>3.24</v>
+      </c>
+      <c r="C31" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <v>3.24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1287,17 +1357,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>63</v>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1.3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1.4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1345,6 +1482,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1581,26 +1737,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1617,22 +1772,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
10 Apr 2025 Update
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5AFF306-D9B4-41BB-996F-F9B64FE9B157}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BF8218-CF47-4461-8424-6EE7B84F4985}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="1260" windowWidth="19035" windowHeight="19230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="1185" windowWidth="19035" windowHeight="19230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>Formation enter</t>
   </si>
@@ -331,6 +331,30 @@
   </si>
   <si>
     <t>Upper completions</t>
+  </si>
+  <si>
+    <t>3.23.4</t>
+  </si>
+  <si>
+    <t>3.23.5</t>
+  </si>
+  <si>
+    <t>Chenge colors in chartView.py to black</t>
+  </si>
+  <si>
+    <t>Make sure planned is not shown in chartView.py if actual exists</t>
+  </si>
+  <si>
+    <t>Why does MD vs TVD show a line back to zero when more than one lateral?</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>3.2.4</t>
+  </si>
+  <si>
+    <t>Add button to export</t>
   </si>
 </sst>
 </file>
@@ -981,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058DFC1C-49F3-4496-A186-6E8CEF18F5C9}">
-  <dimension ref="A2:N31"/>
+  <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,29 +1095,17 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8">
-        <v>3.4</v>
-      </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
       </c>
       <c r="N8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9">
-        <v>3.5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
-      </c>
       <c r="N9" t="s">
         <v>52</v>
       </c>
@@ -1103,10 +1115,10 @@
         <v>61</v>
       </c>
       <c r="B10">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="L10" t="s">
         <v>30</v>
@@ -1120,10 +1132,10 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
         <v>57</v>
@@ -1134,10 +1146,10 @@
         <v>61</v>
       </c>
       <c r="B12">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
         <v>58</v>
@@ -1148,10 +1160,10 @@
         <v>61</v>
       </c>
       <c r="B13">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="L13" t="s">
         <v>30</v>
@@ -1165,44 +1177,47 @@
       <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1">
-        <v>3.1</v>
+      <c r="B14">
+        <v>3.8</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>3.11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>66</v>
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>3.9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
-      <c r="B16">
-        <v>3.12</v>
+      <c r="B16" s="1">
+        <v>3.1</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17">
-        <v>3.13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
+        <v>102</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,10 +1225,10 @@
         <v>61</v>
       </c>
       <c r="B18">
-        <v>3.14</v>
+        <v>3.12</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,10 +1236,10 @@
         <v>61</v>
       </c>
       <c r="B19">
-        <v>3.15</v>
+        <v>3.13</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,10 +1247,10 @@
         <v>61</v>
       </c>
       <c r="B20">
-        <v>3.16</v>
+        <v>3.14</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1243,10 +1258,10 @@
         <v>61</v>
       </c>
       <c r="B21">
-        <v>3.17</v>
+        <v>3.15</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1254,10 +1269,10 @@
         <v>61</v>
       </c>
       <c r="B22">
-        <v>3.18</v>
+        <v>3.16</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1265,21 +1280,21 @@
         <v>61</v>
       </c>
       <c r="B23">
-        <v>3.19</v>
+        <v>3.17</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1">
-        <v>3.2</v>
+      <c r="B24">
+        <v>3.18</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,53 +1302,68 @@
         <v>61</v>
       </c>
       <c r="B25">
-        <v>3.21</v>
+        <v>3.19</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26">
-        <v>3.22</v>
+      <c r="B26" s="1">
+        <v>3.2</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
       <c r="B27">
-        <v>3.23</v>
+        <v>3.21</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
+      <c r="B28">
+        <v>3.22</v>
+      </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29">
+        <v>3.23</v>
+      </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
         <v>87</v>
@@ -1343,11 +1373,57 @@
       <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="B31">
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35">
         <v>3.24</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C35" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>3.25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
   <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1482,25 +1558,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1737,25 +1794,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1772,4 +1830,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
11 Apr 2025 Update FInish Dirrectional section start well builder
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wscsurtech\OneDrive - ConocoPhillips\Surveillance Technician\Tech Folders\Nick\DT\DT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{CBBC392C-310E-471F-983D-11E338F0BAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BF8218-CF47-4461-8424-6EE7B84F4985}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="1185" windowWidth="19035" windowHeight="19230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="1545" windowWidth="28170" windowHeight="19230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
   <si>
     <t>Formation enter</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>Add button to export</t>
+  </si>
+  <si>
+    <t>hole size</t>
+  </si>
+  <si>
+    <t>casing od</t>
+  </si>
+  <si>
+    <t>casing id</t>
+  </si>
+  <si>
+    <t>casing weight</t>
+  </si>
+  <si>
+    <t>casing top</t>
+  </si>
+  <si>
+    <t>casing bottom</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058DFC1C-49F3-4496-A186-6E8CEF18F5C9}">
   <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -1433,15 +1451,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1449,55 +1467,73 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1.2</v>
       </c>
       <c r="D4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1.3</v>
       </c>
       <c r="D5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1.4</v>
       </c>
       <c r="D6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1.5</v>
       </c>
       <c r="D7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>3</v>
       </c>
@@ -1505,7 +1541,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>4</v>
       </c>
@@ -1795,6 +1831,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
@@ -1802,15 +1847,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1833,6 +1869,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1840,12 +1884,4 @@
     <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
14 Apr 2025 Update
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wscsurtech\OneDrive - ConocoPhillips\Surveillance Technician\Tech Folders\Nick\DT\DT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF4C420-FD2F-4DEF-94D1-7A8E7E2A4A1B}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="1545" windowWidth="28170" windowHeight="19230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2850" windowWidth="22290" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
   <si>
     <t>Formation enter</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>casing bottom</t>
+  </si>
+  <si>
+    <t>caing grade</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1457,7 @@
   <dimension ref="B2:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,6 +1542,9 @@
       </c>
       <c r="C9" t="s">
         <v>90</v>
+      </c>
+      <c r="O9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -1594,6 +1600,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1830,26 +1855,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1866,22 +1890,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
16 Apr 25 Changes Add Casing Window Updates
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF4C420-FD2F-4DEF-94D1-7A8E7E2A4A1B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA66AC7-47DB-425C-B230-3555E87FB91F}"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="2850" windowWidth="22290" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
   <si>
     <t>Formation enter</t>
   </si>
@@ -376,6 +376,18 @@
   </si>
   <si>
     <t>caing grade</t>
+  </si>
+  <si>
+    <t>Remove Casing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit button save into database </t>
+  </si>
+  <si>
+    <t>Update casing info based on casing selected</t>
+  </si>
+  <si>
+    <t>Change casing</t>
   </si>
 </sst>
 </file>
@@ -1454,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
-  <dimension ref="B2:O10"/>
+  <dimension ref="B2:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,33 +1538,65 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-      <c r="O8" t="s">
-        <v>110</v>
+      <c r="C8">
+        <v>1.6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="O9" t="s">
-        <v>111</v>
+      <c r="C9">
+        <v>1.7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="O11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1600,25 +1644,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1855,25 +1880,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1890,4 +1916,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
17 Apr 25 Changes, work on well schematic window.
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA66AC7-47DB-425C-B230-3555E87FB91F}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5865D46C-BA2B-4530-A97D-28A09F3864A6}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2850" windowWidth="22290" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="1200" windowWidth="29550" windowHeight="18465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
   <si>
     <t>Formation enter</t>
   </si>
@@ -384,10 +384,31 @@
     <t xml:space="preserve">Submit button save into database </t>
   </si>
   <si>
-    <t>Update casing info based on casing selected</t>
-  </si>
-  <si>
     <t>Change casing</t>
+  </si>
+  <si>
+    <t>update drawing after adding casing</t>
+  </si>
+  <si>
+    <t>why does it say a casing already exists</t>
+  </si>
+  <si>
+    <t>Add conductor</t>
+  </si>
+  <si>
+    <t>Update casing info window based on casing in database</t>
+  </si>
+  <si>
+    <t>find way to order casing correctly in database (surf-&gt;int-&gt;liner-&gt;prod-&gt;tubing)</t>
+  </si>
+  <si>
+    <t>clear canvas somehow?</t>
+  </si>
+  <si>
+    <t>draw packer with liners and tubing</t>
+  </si>
+  <si>
+    <t>Show formation depths</t>
   </si>
 </sst>
 </file>
@@ -1466,15 +1487,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
-  <dimension ref="B2:O14"/>
+  <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1482,7 +1503,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1.1000000000000001</v>
       </c>
@@ -1493,7 +1514,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1.2</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1.3</v>
       </c>
@@ -1515,7 +1536,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1.4</v>
       </c>
@@ -1526,7 +1547,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1.5</v>
       </c>
@@ -1537,7 +1558,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>1.6</v>
       </c>
@@ -1545,15 +1566,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1.7</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
       <c r="B10">
         <v>2</v>
       </c>
@@ -1564,7 +1588,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
       <c r="B11">
         <v>3</v>
       </c>
@@ -1575,7 +1602,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
       <c r="B12">
         <v>4</v>
       </c>
@@ -1583,7 +1613,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
       <c r="B13">
         <v>5</v>
       </c>
@@ -1591,12 +1624,74 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16">
+        <v>7.1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1644,6 +1739,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1880,26 +1994,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1916,22 +2029,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
18 Apr 25 Changes, well builder updates
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5865D46C-BA2B-4530-A97D-28A09F3864A6}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46630EEC-9C93-4A22-A549-FF1D4727480B}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1200" windowWidth="29550" windowHeight="18465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7755" yWindow="630" windowWidth="29550" windowHeight="18465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>Formation enter</t>
   </si>
@@ -409,6 +409,24 @@
   </si>
   <si>
     <t>Show formation depths</t>
+  </si>
+  <si>
+    <t>Generate tubing info database</t>
+  </si>
+  <si>
+    <t>Liner pulls from tubdata nd csgdata for sizes</t>
+  </si>
+  <si>
+    <t>Casing info on left side</t>
+  </si>
+  <si>
+    <t>formations on right side</t>
+  </si>
+  <si>
+    <t>company, well name, and api on top</t>
+  </si>
+  <si>
+    <t>remove casing button</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083C33B9-166D-4730-B1F2-AC8E190260AF}">
-  <dimension ref="A2:O21"/>
+  <dimension ref="A2:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1672,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
       <c r="B17">
         <v>8</v>
       </c>
@@ -1662,7 +1683,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
       <c r="B18">
         <v>9</v>
       </c>
@@ -1670,7 +1694,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
       <c r="B19">
         <v>10</v>
       </c>
@@ -1678,7 +1705,10 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
       <c r="B20">
         <v>11</v>
       </c>
@@ -1686,12 +1716,63 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1739,25 +1820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -1994,25 +2056,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2029,4 +2092,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
19 Apr 25 Changes, finish well builder, find and fix some bugs
</commit_message>
<xml_diff>
--- a/To Do.xlsx
+++ b/To Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://conocophillips.sharepoint.com/sites/ERDRealTimeOperatingCenter-SurveillanceTechnician/Shared Documents/Surveillance Technician/Tech Folders/Nick/DT/DT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46630EEC-9C93-4A22-A549-FF1D4727480B}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{6A6A898C-4050-4595-85B3-801206A0F258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{782EA2A0-FCC0-464C-915D-BBA7C6BF75B7}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="630" windowWidth="29550" windowHeight="18465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33525" yWindow="1665" windowWidth="29550" windowHeight="18465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Need" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="129">
   <si>
     <t>Formation enter</t>
   </si>
@@ -1508,7 +1508,7 @@
   <dimension ref="A2:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,6 +1643,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
       <c r="B14">
         <v>6</v>
       </c>
@@ -1717,6 +1720,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
       <c r="B21">
         <v>12</v>
       </c>
@@ -1736,6 +1742,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
       <c r="B23">
         <v>14</v>
       </c>
@@ -1744,6 +1753,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
       <c r="B24">
         <v>15</v>
       </c>
@@ -1752,6 +1764,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
       <c r="B25">
         <v>16</v>
       </c>
@@ -1760,6 +1775,9 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
       <c r="B26">
         <v>17</v>
       </c>
@@ -1768,6 +1786,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
       <c r="B27">
         <v>18</v>
       </c>
@@ -1820,6 +1841,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038D3AC4C923D914AADDD59032731B02F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40924a8d775008c8bbed94f92c13cccc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea951dc9-54de-426a-a3bb-e5574035f2c6" xmlns:ns3="1f19bc02-2c2d-4d8c-aba0-70a3939b7839" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c007e2d3a945616463f310ac639e4e8" ns2:_="" ns3:_="">
     <xsd:import namespace="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
@@ -2056,26 +2096,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ea951dc9-54de-426a-a3bb-e5574035f2c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A997B4-500A-49A9-89A7-792917B62D0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2092,22 +2131,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{247B784E-B76D-4318-A011-ED25733527B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15FA8EEF-DD6C-4819-A7CF-1C2AED1926F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ea951dc9-54de-426a-a3bb-e5574035f2c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>